<commit_message>
fsos remove target; updated with test scene type
</commit_message>
<xml_diff>
--- a/Projects/TWEGAU/Data/setup.xlsx
+++ b/Projects/TWEGAU/Data/setup.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
-    <t xml:space="preserve">Fridge Door, Floor Display</t>
+    <t xml:space="preserve">cold space SOS – Scene01</t>
   </si>
   <si>
     <t xml:space="preserve">Include </t>
@@ -277,24 +277,24 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.62755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.8826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.4591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.3775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.4591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="29.0765306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="21.9948979591837"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="15.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.9387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="28.7551020408163"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
update template to fix scene name with unicode
</commit_message>
<xml_diff>
--- a/Projects/TWEGAU/Data/setup.xlsx
+++ b/Projects/TWEGAU/Data/setup.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
-    <t xml:space="preserve">cold space SOS – Scene01</t>
+    <t xml:space="preserve">cold space SOS - Scene01</t>
   </si>
   <si>
     <t xml:space="preserve">Include </t>
@@ -277,24 +277,24 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-12476 TWEGAU Template change SceneType addition
</commit_message>
<xml_diff>
--- a/Projects/TWEGAU/Data/setup.xlsx
+++ b/Projects/TWEGAU/Data/setup.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
-    <t xml:space="preserve">cold space SOS - Scene01</t>
+    <t xml:space="preserve">Fridge Door,Impulse Fridge,Open Fridge,Standalone Fridge,TWE Standalone Fridge</t>
   </si>
   <si>
     <t xml:space="preserve">Include </t>
@@ -277,14 +277,14 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.95"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.1479591836735"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.530612244898"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.1428571428571"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.1173469387755"/>

</xml_diff>